<commit_message>
trab en la U
02_01_19
</commit_message>
<xml_diff>
--- a/proj.abejas/data.xlsx
+++ b/proj.abejas/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\YulianaElizabeth\Desktop\fotos tesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proy_GitHub_DH\r_script_dh\proj.abejas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
     <sheet name="Hoja4" sheetId="7" r:id="rId7"/>
     <sheet name="Hoja5" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="90">
   <si>
     <t xml:space="preserve">Concentración de plomo </t>
   </si>
@@ -231,15 +231,6 @@
     <t>Cuenca</t>
   </si>
   <si>
-    <t xml:space="preserve">Mes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variable </t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
     <t>UDA</t>
   </si>
   <si>
@@ -299,13 +290,25 @@
   <si>
     <t>polen</t>
   </si>
+  <si>
+    <t>setor</t>
+  </si>
+  <si>
+    <t>mes</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -383,15 +386,15 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,7 +413,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -449,7 +452,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -475,7 +477,7 @@
               <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -563,6 +565,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A815-4329-9352-EDB020510E02}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -641,6 +648,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A815-4329-9352-EDB020510E02}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -719,6 +731,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A815-4329-9352-EDB020510E02}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -788,7 +805,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462183968"/>
@@ -847,7 +864,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462193216"/>
@@ -874,7 +891,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -900,7 +916,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -930,7 +946,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -942,7 +958,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -981,7 +997,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1007,7 +1022,7 @@
               <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1095,6 +1110,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3B0D-4A08-84BB-A08C6C57BC61}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1173,6 +1193,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3B0D-4A08-84BB-A08C6C57BC61}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1251,6 +1276,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3B0D-4A08-84BB-A08C6C57BC61}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1320,7 +1350,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462188864"/>
@@ -1379,7 +1409,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462186144"/>
@@ -1406,7 +1436,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1432,7 +1461,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1462,7 +1491,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1474,7 +1503,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1518,7 +1547,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1544,7 +1572,7 @@
               <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1609,6 +1637,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6871-4478-870E-4BDCB9AE398D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1678,7 +1711,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462187232"/>
@@ -1737,7 +1770,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462187776"/>
@@ -1788,7 +1821,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1800,7 +1833,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1844,7 +1877,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1870,7 +1902,7 @@
               <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1940,6 +1972,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-45CF-4B21-A4C3-E3C918BC7E2F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2000,6 +2037,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-45CF-4B21-A4C3-E3C918BC7E2F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2060,6 +2102,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-45CF-4B21-A4C3-E3C918BC7E2F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2129,7 +2176,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462183424"/>
@@ -2188,7 +2235,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462192128"/>
@@ -2215,7 +2262,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2241,7 +2287,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2271,7 +2317,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2283,7 +2329,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2327,7 +2373,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2353,7 +2398,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2412,6 +2457,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4799-4FB9-A200-CAD2D9CB64D3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2467,7 +2517,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462181248"/>
@@ -2526,7 +2576,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462190496"/>
@@ -2567,7 +2617,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2579,7 +2629,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2648,7 +2698,7 @@
               <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2743,6 +2793,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-182C-43E3-BE78-12C123C7FB6D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2812,7 +2867,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462185600"/>
@@ -2871,7 +2926,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1462180160"/>
@@ -2922,7 +2977,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2934,7 +2989,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2998,7 +3053,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3063,6 +3118,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6017-4D03-824F-0BFEF90512AC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3118,7 +3178,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1355902528"/>
@@ -3177,7 +3237,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1593684720"/>
@@ -3218,7 +3278,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3230,7 +3290,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -3289,7 +3349,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3407,6 +3467,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C87D-4AFF-B3E0-09CCB157FF82}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3515,6 +3580,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C87D-4AFF-B3E0-09CCB157FF82}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3623,6 +3693,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C87D-4AFF-B3E0-09CCB157FF82}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3675,7 +3750,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1355899808"/>
@@ -3731,7 +3806,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1355896000"/>
@@ -3771,7 +3846,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3801,7 +3876,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8900,17 +8975,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -9524,7 +9599,7 @@
       <c r="D6" s="3">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <f t="shared" si="0"/>
         <v>4.8666666666666671E-2</v>
       </c>
@@ -9593,7 +9668,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B2" s="4">
         <v>7.4999999999999997E-2</v>
@@ -9848,7 +9923,7 @@
       <c r="D3" s="3">
         <v>0.26</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <f t="shared" ref="E3:E4" si="0">AVERAGE(B3:D3)</f>
         <v>0.23433333333333331</v>
       </c>
@@ -9866,7 +9941,7 @@
       <c r="D4" s="3">
         <v>0.41</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <f t="shared" si="0"/>
         <v>0.24766666666666662</v>
       </c>
@@ -10219,658 +10294,658 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E47"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:B47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="9" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="D20" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B22" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="B23" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="3">
+      <c r="B26" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="4">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B30" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="B35" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="4">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="B37" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="3">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B44" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B45" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="4">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0.115</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="4">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="4">
-        <v>0.105</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="4">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="4">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="4">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="4">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="4">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="4">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E36" s="4">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E37" s="4">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E38" s="4">
-        <v>1.6E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
+      <c r="B46" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" s="3">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="3">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E41" s="3">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E43" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="3">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" s="3">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" s="3">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E47" s="3">
+      <c r="C46" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="3">
         <v>0.41</v>
       </c>
     </row>
@@ -10882,201 +10957,201 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:F18"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="3">
+      <c r="B2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="3">
         <f>Miel!E2</f>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="3">
         <f>Miel!E3</f>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" s="3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="3">
         <f>Miel!E4</f>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="3">
         <f>Miel!E5</f>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="12">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="11">
         <f>Miel!E6</f>
         <v>4.8666666666666671E-2</v>
       </c>
     </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="3">
         <f>Miel!E7</f>
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="4">
         <f>Polen!E2</f>
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="4">
         <f>Polen!E3</f>
         <v>7.166666666666667E-2</v>
       </c>
     </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="4">
         <f>Polen!E4</f>
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="4">
         <f>Polen!E5</f>
         <v>3.5333333333333335E-2</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="4">
         <f>Polen!E6</f>
         <v>5.2666666666666667E-2</v>
       </c>
     </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" s="4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="4">
         <f>Polen!E7</f>
         <v>4.1333333333333333E-2</v>
       </c>
     </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="3">
         <f>Mp!E2</f>
         <v>0.68099999999999994</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="12">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="11">
         <f>Mp!E3</f>
         <v>0.23433333333333331</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="12">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="11">
         <f>Mp!E4</f>
         <v>0.24766666666666662</v>
       </c>

</xml_diff>